<commit_message>
Added code fix and logging
</commit_message>
<xml_diff>
--- a/reports/Bill_Statement.xlsx
+++ b/reports/Bill_Statement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,342 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vanilla Cream</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8750</v>
+      </c>
+      <c r="D2" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Filter Coffee</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2700</v>
+      </c>
+      <c r="D3" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cold Coffee</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D4" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Black Coffee</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>880</v>
+      </c>
+      <c r="D5" t="n">
+        <v>70.40000000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Normal Tea</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>250</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lemon Tea</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>350</v>
+      </c>
+      <c r="D7" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ginger Tea</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D8" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Honey Tea</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>405</v>
+      </c>
+      <c r="D9" t="n">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bhel Puri</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2200</v>
+      </c>
+      <c r="D10" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sev Puri</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D11" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Peanut Masala</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2990</v>
+      </c>
+      <c r="D12" t="n">
+        <v>358.8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Chilli Cheese</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3450</v>
+      </c>
+      <c r="D13" t="n">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Chicken Tikki</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2980</v>
+      </c>
+      <c r="D14" t="n">
+        <v>536.4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kheema chat</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="D15" t="n">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Shambi Kabab</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3750</v>
+      </c>
+      <c r="D16" t="n">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Chicken Tandoor</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3400</v>
+      </c>
+      <c r="D17" t="n">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Veggie Delite</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D18" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Paneer Tikka</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2750</v>
+      </c>
+      <c r="D19" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Corn n Peas</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1750</v>
+      </c>
+      <c r="D20" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Peri Peri Chicken</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3350</v>
+      </c>
+      <c r="D21" t="n">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ham Chicken</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3250</v>
+      </c>
+      <c r="D22" t="n">
+        <v>585</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added enhanced/fixed streamlit codes
</commit_message>
<xml_diff>
--- a/reports/Bill_Statement.xlsx
+++ b/reports/Bill_Statement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,331 +464,355 @@
       <c r="B2" t="n">
         <v>50</v>
       </c>
-      <c r="C2" t="n">
-        <v>8750</v>
-      </c>
-      <c r="D2" t="n">
-        <v>700</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>8750.00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>700.0000</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Filter Coffee</t>
+          <t>Latte</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2700</v>
-      </c>
-      <c r="D3" t="n">
-        <v>216</v>
+        <v>20</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>160.0000</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cold Coffee</t>
+          <t>Filter Coffee</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D4" t="n">
-        <v>144</v>
+        <v>30</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2700.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>216.0000</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Black Coffee</t>
+          <t>Cold Coffee</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>880</v>
-      </c>
-      <c r="D5" t="n">
-        <v>70.40000000000001</v>
+        <v>12</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1800.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>144.0000</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Normal Tea</t>
+          <t>Black Coffee</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>10</v>
       </c>
-      <c r="C6" t="n">
-        <v>250</v>
-      </c>
-      <c r="D6" t="n">
-        <v>20</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>880.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>70.4000</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lemon Tea</t>
+          <t>Normal Tea</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>10</v>
       </c>
-      <c r="C7" t="n">
-        <v>350</v>
-      </c>
-      <c r="D7" t="n">
-        <v>28</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>250.00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20.0000</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ginger Tea</t>
+          <t>Lemon Tea</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>10</v>
       </c>
-      <c r="C8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D8" t="n">
-        <v>32</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>350.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>28.0000</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Honey Tea</t>
+          <t>Ginger Tea</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>10</v>
       </c>
-      <c r="C9" t="n">
-        <v>405</v>
-      </c>
-      <c r="D9" t="n">
-        <v>32.4</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>400.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>32.0000</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bhel Puri</t>
+          <t>Honey Tea</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>10</v>
       </c>
-      <c r="C10" t="n">
-        <v>2200</v>
-      </c>
-      <c r="D10" t="n">
-        <v>264</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>405.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>32.4000</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sev Puri</t>
+          <t>Bhel Puri</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>10</v>
       </c>
-      <c r="C11" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D11" t="n">
-        <v>204</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2200.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>264.0000</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peanut Masala</t>
+          <t>Sev Puri</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>10</v>
       </c>
-      <c r="C12" t="n">
-        <v>2990</v>
-      </c>
-      <c r="D12" t="n">
-        <v>358.8</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1700.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>204.0000</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chilli Cheese</t>
+          <t>Aloo Tikki</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>10</v>
       </c>
-      <c r="C13" t="n">
-        <v>3450</v>
-      </c>
-      <c r="D13" t="n">
-        <v>414</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2800.00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>336.0000</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chicken Tikki</t>
+          <t>Peanut Masala</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>10</v>
       </c>
-      <c r="C14" t="n">
-        <v>2980</v>
-      </c>
-      <c r="D14" t="n">
-        <v>536.4</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2990.00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>358.8000</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kheema chat</t>
+          <t>Chilli Cheese</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>10</v>
       </c>
-      <c r="C15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D15" t="n">
-        <v>558</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3450.00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>414.0000</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Shambi Kabab</t>
+          <t>Chicken Tikki</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>10</v>
       </c>
-      <c r="C16" t="n">
-        <v>3750</v>
-      </c>
-      <c r="D16" t="n">
-        <v>675</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2980.00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>536.4000</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chicken Tandoor</t>
+          <t>Kheema chat</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>10</v>
       </c>
-      <c r="C17" t="n">
-        <v>3400</v>
-      </c>
-      <c r="D17" t="n">
-        <v>612</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3100.00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>558.0000</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Veggie Delite</t>
+          <t>Shambi Kabab</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>10</v>
       </c>
-      <c r="C18" t="n">
-        <v>2500</v>
-      </c>
-      <c r="D18" t="n">
-        <v>300</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3750.00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>675.0000</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Paneer Tikka</t>
+          <t>Chicken Tandoor</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>10</v>
       </c>
-      <c r="C19" t="n">
-        <v>2750</v>
-      </c>
-      <c r="D19" t="n">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Corn n Peas</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>10</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1750</v>
-      </c>
-      <c r="D20" t="n">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Peri Peri Chicken</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>10</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3350</v>
-      </c>
-      <c r="D21" t="n">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Ham Chicken</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" t="n">
-        <v>3250</v>
-      </c>
-      <c r="D22" t="n">
-        <v>585</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3400.00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>612.0000</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>